<commit_message>
feat: extract texts from links
</commit_message>
<xml_diff>
--- a/chip-in.asia.xlsx
+++ b/chip-in.asia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>URL</t>
   </si>
@@ -22,48 +22,72 @@
     <t>Page Title</t>
   </si>
   <si>
+    <t>Page Content</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/</t>
   </si>
   <si>
     <t>CHIP - The Ultimate Digital Finance Platform for Your Business</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowTHE ULTIMATE —Digital Finance Platform for Your BusinessDigitize, Simplify, and Accelerate Your Financial Management Processes Today!Start Your Digital Finance JourneyTrusted by Top Brandsand more...INTRODUCTIONTransform Your Financial Management with CHIPCHIP stands at the forefront of the digital finance revolution, empowering MSMEs with our integrated platform.We have evolved from providing e-commerce infrastructure to digitize the financial processes at the heart of your business.Now, CHIP simplifies and accelerates everything from payment collection to risk management, tailored perfectly for modern merchants.Our mission is to take your business to greater heightsWe started by offering merchants a better way to accept payments online, but we didn't stop there!We know that every business of all sizes has different needs, so we've created products that let you choose what works best financially for your company and help you get more profit than ever before.CHIP MODULESModular Digital Finance Solutions, Designed for Your SuccessPower to manage and optimize your business's financial operations across four main pillars:COLLECTSimplify your payment processesReceive funds online and OTC via multiple payment methods securely &amp; effortlessly.Learn moreCONTROLComplete visibility over expensesWe help you manage everything from sending funds to handling petty cash.CHIP SendCHIP ExpenseCOMPLIANCEProtect your businessOur service helps identify, assess, and mitigate financial risks to ensure peace of mind.Learn moreCOINStreamline treasury managementEffortlessly roll collection funds into money market opportunities.Learn moreWhy should CHIP be your payment solution for all businessesStart-up FriendlyNew businesses without track record can still accept collection via multiple payment methods.Flexible Settlement &amp; PayoutCustomise your settlement speed, flow and methodsZero Setup FeeStart collecting customer payments without initial and monthly feeCollect &amp; GrowWe don't stop helping you collect customer payments. We also help you earn more from the collection, manage expenses &amp; ensure compliance.Want to scale your business? Let us help you!Our all-in-one payment solution is ready to serve you!Collect via customizable invoices, links, and online terminalsZero upfront payment, credit reloads and minimum collection amountCustomisable Secured PageOpt for customizable transactional rates &amp; settlement speedFocus on online-to-offline, recurring &amp; cross-border paymentsCollect recurring payments for your businessReconcile, analyze and project collection for every campaignComing soonConnect with accounting softwares and e-Commerce platformsComing soonDistribute payouts to multiple bank accounts or other CHIP modules in real-time from your collected funds.BETAAS FEATURED ONWe aim to contribute to your growth!CHIP can be used by any business of any size to make fast, secure payments.Your business is growing, and we want to help you get there!New Sellers / BusinessesSMEsDevelopersWhether you’re a street vendor or home-based business owner, our services can be tailored to meet your needs.Learn moreReady to Digitize Your Financial Management?Join other growing businesses that have transformed their financial processes with CHIP. Start your journey towards more efficient, transparent, and powerful financial management today.Get Started with CHIPContact usDrop any questions in the form below, and we will reach out to you soon!or call our office lineNeed a support? Email us at support@chip-in.asiaFull nameOrganization / Company nameEmailContact number(Eg: +60123456778 or +60345678910)Interest(s)MerchantPartnershipReferrerOtherPreferred communication method(s)By emailBy phone callBy TelegramSubmitCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"17f3c960b1e7ba54ab9a221baf1abf6a-2b9f95a18c2d4475-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=17f3c960b1e7ba54ab9a221baf1abf6a,sentry-sample_rate=1,sentry-transaction=GET%20%2F,sentry-sampled=true"}},"page":"/","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/collect</t>
   </si>
   <si>
     <t>CHIP Collect - Accept payment online or over-the-counter</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowCOLLECTAccept payment online or over-the-counter with CHIP CollectWhether you run your business on a website, social media or from a physical store - we have solutions to fit your needs.Start Collecting Payments NowContact salesCHIP Collect super powersWe design our solutions to let you focus on running and growing your business.Powerful Dashboard &amp; AnalyticsAssign specific roles for teamInitiate refund easilyToggle easily between staging &amp; production environmentFast approvalEasy-to-setup recurring paymentAccept cross-border paymentsCustomisable Secured Payment PageSecurity and complianceWe put security and scalability above everything else. We bring together best practices and technologies to ensure a safe &amp; reliable platform for our merchants.ISO/IEC 27017:2015CertifiedISO/IEC 27001:2022‍CertifiedPCI-DSS‍Level 1 compliantPowered by AWSOur payment stacksMaximise your collection and revenue with smarter tools.Consolidate on-premise &amp; online collection + cross-border payments (future)Reconcile, analyze and project collection for every campaignCollect via customizable invoices, links and terminalsConnect with accounting software and e-Commerce platformsSplit settlement to multiple bank accounts and/or other CHIP modulesOpt for customized settlement speed &amp; transactional ratesFee and SettlementOur fee and settlement is tailored for businesses of every sizes.FPX Online BankingThe most popular online payment methods in Malaysia. Collect payment from individual customers (FPX B2C) &amp; corporate client (FPX B2B1).B2C &amp; B2B1B2C Fee:RM1*B2B1 Fee:RM2*Settlement:Every next day**Local credit and debit cardsCollect online payment from Malaysian customers who prefer to pay using credit, debit or prepaid cards.Credit card:2.0%*Debit card:1.0%*Recurring payments:AvailableSettlement:Every 2 business days*On-Premise POS TerminalAccept payments at your physical store using a point of sale terminal./Local Credit Card:1.35%*Local Debit Card:1.00%*Foreign Card:4.40%*Touch 'n Go:0.95%*GrabPay:1.05%*Boost:1.00%*ShopeePay:1.15%*Maybank QRPay:0.95%*Alipay:1.00%*UnionPay QR:1.80%*Settlement:Every 2 business days*Foreign credit and debit cardsCollect card payment online from customers globally.Credit card:3.0%*Debit card:1.8%*Recurring payments:AvailableSettlement:Every 2 business days*E-walletsCollect online payment from customers who prefer to pay using e-wallets.All E-wallets:1.40%*Settlement:Every 2 business days*Buy Now, Pay LaterAllow customer to make purchases today and pay them at future dates.Atome:5.3%*Settlement:Every Thursday of the following week*DuitNow QR (Online)Collect payment from customers who opt to scan digital QR codes – including support for cross-border QR payments, ideal for international customers from Indonesia, Thailand and Singapore. Learn more/DuitNow QR (Online):1.60%(Minimum: RM0.15, Maximum: RM1.50)*Settlement:Every Next Day**DuitNow Online Banking &amp; Auto-DebitCollect online payment from individuals &amp; corporate client.Coming Soon* Subject to final approval.** The time required for funds to reach a bank account is dependent on the bank's operating hours and system uptime.Merchants’ use casesCHIP Collect can be used by any business of any size to collect fast, secure payments.With Website / AppEasy-to-use APIMultiple librariesReady webhookiOS &amp; Android SDKsReady checkout plugins:WooCommerceWooCommerce SubscriptionsWooCommerce One Page CheckoutGiveWPFluent FormsGravity FormsWHMCSAffiliateWPAbanteCartCharitableWP Car RentalWithout Website / AppCustomizable payment linkDonation featureSocial media enabledQuick invoicingOnline Sales Platform Partners:EasyStoreOnPayOrderla.myShoppegramFighterFounderHQAdsHelperBverrWhatsMenuWasep.meClientExecWith Physical OutletReady terminal to accept QR and cardConsolidated reporting between outlet &amp; online salesYour favourite plugins 🤝 CHIPSuper charge your online store with CHIP-compatible plugins.How it works?We simplify the complex processes in every payment flow.Need an access to a test account?Register for free now and toggle between testing and actual portals easily!Start Collecting Payments NowContact usDrop any questions in the form below, and we will reach out to you soon!or call our office lineNeed a support? Email us at support@chip-in.asiaFull nameOrganization / Company nameEmailContact number(Eg: +60123456778 or +60345678910)Interest(s)MerchantPartnershipReferrerOtherPreferred communication method(s)By emailBy phone callBy TelegramSubmitCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"eb05591bf2fd2a346701f6fd286ee77b-6517ba86038aca6d-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=eb05591bf2fd2a346701f6fd286ee77b,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcollect,sentry-sampled=true"}},"page":"/collect","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/control/send</t>
   </si>
   <si>
     <t>CHIP Send - Empower local payouts in real-time</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart Now CHIP SendBetaEmpower local payouts in real-timeTransact with confidence. Send payouts immediately to any organisations and individuals.Dive into our APIContact usNo-code Coming SoonHow it works?STEP 1Allocate Budget from Daily CollectionSTEP 2Add Recipients &amp; Real-time Bank Account VerificationSTEP 3Initiate Real-time Payouts with Send APISTEP 4Manage Budget &amp; Monitor Payout StatusCollect SendSEAMLESS PAYOUTSAllocate Budget from Daily CollectionsEliminating reload delays and inefficiencies.SECURED PAYOUTSUnwavering Commitment to Security &amp; ComplianceAt CHIP, we go beyond mere transactions; we're committed to preserving trust amid complex regulations. We prioritize exceeding requirements, safeguarding merchants' interests, and ensuring seamless operations.To deliver on this promise, CHIP Send includes:Record Payout DetailsFor every payout, set a unique reference. Whether you want a broad overview or a detailed description, tailor each payout’s specifics to your needs.Beneficiary Bank Account VerificationDon't leave things to chance. With our advanced API, you can verify the status of any bank account in real-time, ensuring your funds are directed towards valid and active accounts.Approver RulesFlexibility at its finest. Establish dynamic approver protocols, whether it’s a one-of-two approval system or a stringent two-out-of-two agreement.Approver FlowsEmpower your operations by designating one or multiple individuals for approval of payout budget allocations.Real-Time Status UpdatesReceive instant notifications on the status of every payout, keeping you informed in the moment with our reliable webhooks.No-code Coming SoonCHIP SendDesigned for Multifaceted Payout ScenariosIn the fast-paced digital world, every business is different. That's why we created CHIP Send, a solution designed to handle various payout needs. No matter what your business requires, we've got it covered.Here are just a few ways you can leverage CHIP Send:WithdrawalsSeamless and swift, CHIP Send facilitates efficient withdrawals, reducing wait times and enhancing user satisfaction.Agents CommissionRewarding your agents is a breeze. With CHIP Send, commissions are processed promptly and accurately, ensuring your agents feel valued and motivated.Pay Contract WorkersStreamline payments for freelancers, temporary staff, and remote teams with CHIP Send. Ensure timely payments, simplify processes, and foster trust with your workforce.No matter the use case, CHIP Send is your trusted partner for streamlined and secure payouts.Why use CHIP Send?Efficient Payment ManagementCHIP Send streamlines various payout scenarios, from withdrawals and agents commission to paying contract workers, in real-time!Unwavering Security &amp; ComplianceWith a strong commitment to safety, CHIP Send stays updated with evolving compliance and regulations. This protects merchant interests and guarantees the security of every transaction.Customizable Approver FlowsMerchants can establish tailored approval processes, assigning single or multiple approvers for payout budgets, and setting dynamic rules to fit their organizational needs.Real-time Bank VerificationCHIP Send's API allows for instantaneous bank account verification, ensuring that recipient accounts are active and valid, minimizing transactional errors.Detailed Record KeepingEvery payout can be associated with unique references and descriptions, allowing merchants to maintain clear and organized financial records.Affordable &amp; Transparent PricingCHIP SendVerify multiple individual/organization beneficiaries &amp; initiate payout in real-time using API or no-code portalTransfer Fee:RM1*per successful transferVerification Fee:RM1*per successful bank account verification(one-time)Verification &amp; Settlement:Real-time**Budget allocation fee:FreeWhen you allocate Send budget via CHIP Collect (Collections)RM1*When you allocate Send budget via FPX* Subject to final approval** The time required for funds to reach a bank account is dependent on the bank's operating hours and system uptime.Seamless Integration with CHIP SendWhether you're tech-savvy or not, CHIP Send has got you covered.For DevelopersDive straight into our user-friendly API.Test responses directly on our dedicated API page.Need to experiment?Just request staging credentials, and you're all set.Dive into our Send APIFor the Non-TechiesFret not! We're expanding our horizon to make CHIP Send accessible to everyone:No-Code CHIP Platform Coming SoonMaking payouts simpler than ever, without a single line of code.WordPress Plugins Coming SoonContact usDrop any questions in the form below, and we will reach out to you soon!or call our office lineNeed a support? Email us at support@chip-in.asiaFull nameOrganization / Company nameEmailContact number(Eg: +60123456778 or +60345678910)Interest(s)MerchantPartnershipReferrerOtherPreferred communication method(s)By emailBy phone callBy TelegramSubmitCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"1bb254446f438a8ad9c9cf5a37eb5902-0814329631f63697-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=1bb254446f438a8ad9c9cf5a37eb5902,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcontrol%2Fsend,sentry-sampled=true"}},"page":"/control/send","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/control/expense</t>
   </si>
   <si>
     <t>CHIP Expense - Streamline Your Team's Expense Management</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart Now CHIP ExpenseBetaStreamline Your Team's Expense ManagementCHIP Expense simplifies your expense management with automated tracking, insightful analytics, and seamless integrations.Contact us todayExpense Reporting Made EffortlessWhenever staff incur expenses, you'll receive instant notifications.Just point, click, and upload receipts directly through the app.Review submissions and give your approval with a single touch.ULTIMATE EXPENSE CONTROLKeep Control Over Staff SpendingCHIP Expense ensures that staff spending stays within limits by enabling pre-defined budget allocations.Freeze and allocate funds in real-time and safeguard your business with our comprehensive tools against fraud and overspending.Smart Financial ManagementEnjoy Proactive Spending LimitsSetting up spending limits in CHIP Expense goes beyond mere budgeting. They act as a proactive financial control mechanism, empowering you to manage your team's spending effectively.Assign specific spend limits and vendor constraints effortlessly—no more awkward conversations or micromanagement, just smart control.Empower Your Finances with Streamlined Expense ManagementReal-Time Expense MonitoringGain immediate visibility into all transactions as they populate your dashboard—no more waiting for month-end reports.Simplified Employee ReimbursementManaging out-of-pocket expenses, from petty cash to mileage, is effortless, ensuring your staff are reimbursed quickly and accurately.Expense Approval WorkflowReview transactions to ensure compliance with company policies. Approve or deny expenses with clarity and control.Fraud Protection MechanismsSecure your finances with allocated budgets for each team. Our duplicate detection tool helps prevent fraudulent claims and unauthorized spending.Smart Transaction Categorization  Coming SoonSet rules for amounts, merchants, and budgets to automatically sort expenses. Swift payments with QR, swift categorization.Integrated Accounting Ecosystem  Coming SoonSync CHIP Expense with your accounting software to reflect your chart of accounts, cutting out hours of manual entry for the swiftest monthly close.CHIP's securityWe understand that in order to serve our customers, we have to diligently protect your financial information with industry-leading standards, protocols, and technology.Proactive fraud protectionPCI-DSS Level 1 compliantCloudflare securityPowered by AWSWhy use CHIP Expense?Customize Budgets to Your Business NeedsMaximize your resources by tailoring budgets to specific departments, teams, or projects. Add or remove personnel flexibly to align with your strategic objectives.Fund Allocation Across PlatformsWhether you’re on the go or at your desk, managing budget approvals is just a notification away. Make informed decisions with ease from any device.Real-Time Spending InsightsKeep your finger on the pulse of your finances. Our platform provides a live view of expenditures against budgets, ensuring you’re always informed about your financial position.Detailed Expenditure AnalysisGain valuable insights with detailed reports. Break down spending data by department, team, or individual to make data-driven decisions.Project and Periodic Budget ReviewsEvaluate past expenditures and plan for the future with our budget review tools. Adjust financial forecasts to stay on track with your fiscal goals.Team-Based Budget ManagementEmpower your team leads with the autonomy to manage their own budgets through customized access and control settings.Instant Mobile NotificationsEnable your staff to request funds on demand. Approvals or rejections are just a tap away with instant notifications to your mobile device.Proactive Expenditure ControlsImplement pre-approval for expenses to prevent budget overruns. Ensure every spend is justified and accounted for within your financial strategy.Coming SoonAccelerate Your Reconciliation ProcessBid farewell to the time-consuming task of reconciling credit card and petty cash statements every month.With CHIP Expense, simply scan a QR code and your expenses are automatically categorized and queued for synchronization with your accounting system, ensuring the quickest path to month-end closure.Commonly asked questionsIs this app solely for expense claims, or can businesses also make payments through it?CHIP Expense is a versatile app designed for businesses, functioning as both a payment and an expense claim platform. It allows for easy reloading of funds, invitation of staff members, and swift payments via DuitNow QR, streamlining the replacement of traditional petty cash systems.Will we have to manually enter all our spending from the app into our accounting software?No manual entry is needed. All spending transactions and receipts will soon be able to integrate seamlessly with major accounting software solutions. Integration capabilities are on the horizon. Stay tuned for updates!What is the duration for which transaction and receipt records are stored?We securely retain all transaction records, including attachments, for a period of seven years.Can we synchronize our chart of accounts with the app?Integration with your accounting software to map your chart of accounts with expense categories within the app is in development.  Available SoonWhy does CHIP Expense prefer QR transactions over card payments?Our market research indicates that most MSMEs still process payments in cash, either directly or through petty cash and expense reimbursements. With the growing acceptance of DuitNow QR, many merchants, particularly in retail, are adopting QR as a cost-effective alternative to credit card terminals.Is it possible for accounting or bookkeeping firms to use this app for their clients?Absolutely. Accounting and bookkeeping firms can utilize CHIP Expense as a comprehensive tool to manage their clients' finances. For partnership inquiries or more detailed information, please reach out to our Partnership Manager.Does CHIP Expense support multi-entity management for groups of companies?Yes, CHIP Expense supports an organization-wide framework, allowing administrative users to oversee and manage spending across different entities within a corporate group.Contact usDrop any questions in the form below, and we will reach out to you soon!or call our office lineNeed a support? Email us at support@chip-in.asiaFull nameOrganization / Company nameEmailContact number(Eg: +60123456778 or +60345678910)Interest(s)MerchantPartnershipReferrerOtherPreferred communication method(s)By emailBy phone callBy TelegramSubmitCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"a94b9ef138733305f24364782965341d-c27dcc5e138a9cae-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=a94b9ef138733305f24364782965341d,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcontrol%2Fexpense,sentry-sampled=true"}},"page":"/control/expense","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/control/advance</t>
   </si>
   <si>
     <t>CHIP Advance - Grow your sales with Pay-As-You-Sell Advance™</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart Now CHIP AdvanceIN PARTNERSHIP WITHGrow Your Sales with CHIP AdvanceAn exclusive Shariah-based financing solution for your business, offering a frictionless line of credit that's accessible at all times.Contact our teamHow CHIP Advance works?STEP 1Fill in the form to unlock the offer.STEP 2Submit an advance funds request.STEP 3Receive funds within 48 hours after approval.STEP 4Use the funds to grow your business and repay as your revenue grows.Pay-as-you-sell advance™Access Funds Up to 10x Your Weekly SalesGet instant access to funds based on your sales, with flexible repayment linked directly to your business performance.Repay As You EarnAutomatically Repay from Your Sales, Keeping Cash Flow SimpleEnjoy automatic, hassle-free repayments with no interest or late fees, making cash flow management effortless.Empower Your GrowthFocus on Growing Your Business, Not Managing FinancesWith no interest or late fees, CHIP Advance lets you concentrate on scaling your business, while we take care of the financing.ACHIEVEMENTS UNLOCKED!Total Sales Advance Fund Disbursed To MerchantsMany merchants have leveraged CHIP Advance to access flexible funding and grow their businesses.RM5.0 millionMMAs of August 2025Why use CHIP Advance?No Interest, No Late FeesGet an advance with a one-time fee of 6% and no additional interest charges or late fees, ever.Funds in 48 HoursSubmit your advance request in under 5 minutes and receive funds within 48 hours.Automated, Flexible RepaymentsAutomatically repay through future sales via your settlement partner.Advance Funds Based on SalesYour available advance increases as your sales grow.Certified Shariah-CompliantSeedflex’s Pay-As-You-Sell Advance™️ is certified as Shariah-compliant.Robust SecuritySSL-secured connection for your peace of mind.Frequently Asked QuestionsWho is eligible for CHIP Advance?Merchants must meet basic eligibility criteria, including a consistent sales history. Specific requirements may vary, so contact us to confirm your eligibility.Do I need collateral to qualify?No, CHIP Advance is unsecured financing, meaning you don’t need to provide any assets, like property or equipment, as collateral. Approval is based on your sales performance and business profile.How much funding can I get?The funding amount is determined by your historical sales data. You may qualify for an advance of up to 10 weeks’ worth of sales.Are there any hidden fees or charges?There are no hidden fees. CHIP Advance charges a one-time fee of 6%, with no interest or late fees.How does repayment work?Repayment is fully automated and tied to your sales. A fixed percentage of your daily transactions is deducted until the advance is fully repaid.What happens if my sales slow down?CHIP Advance is designed to adjust with your revenue. If your sales slow down, repayments decrease, minimizing the impact on your business.Register Your InterestFill in the interest form to allow CHIP to share your Company Information with Seedflex to access your available amount.You will receive your login details from Seedflex within 2 business days.Full name*Organization / Company name*Email*Contact number*By checking the box, I consent for CHIP to share my personal information with Seedflex*SubmitCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"b4a867f20bbda72ac20886fa7d1f7369-678177c02a3afe0b-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=b4a867f20bbda72ac20886fa7d1f7369,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcontrol%2Fadvance,sentry-sampled=true"}},"page":"/control/advance","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/compliance</t>
   </si>
   <si>
     <t>CHIP Compliance - Be in compliance with the local regulations while growing</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowCOMPLIANCEComing soonComply with the local regulations while growingKEY FEATURESOnline incorporaton of SDN BHD for sole prop or individual merchantseKYC and online application for business bank account openingSubscribe to accounting, auditing &amp; management reporting servicesCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"19ca05f976175a9d102858fff3f7a92b-c43d4a8a210afe52-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=19ca05f976175a9d102858fff3f7a92b,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcompliance,sentry-sampled=true"}},"page":"/compliance","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/coin</t>
   </si>
   <si>
     <t>CHIP Coin - Earn additional income from your cashflow &amp; collection</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowCOINComing soonEarn additional income from your cashflow &amp; collectionKEY FEATURESEarn profit-shares from CHIP's FD &amp; money market placementSet longer settlement period to maximize returnConnect with accounting software to record incomeCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"a323a866499fbc87b9efbca66a968b35-39517055a92785a3-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=a323a866499fbc87b9efbca66a968b35,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcoin,sentry-sampled=true"}},"page":"/coin","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://blog.chip-in.asia/</t>
   </si>
   <si>
@@ -79,6 +103,9 @@
     <t>Careers at CHIP</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowJoin CHIP A Fintastic Opportunity!We're on a constant quest to redefine the fintech landscape, and we need talented individuals like you to make our dreams a reality. Join our ranks for an unrivaled opportunity to make a difference.Join our teamOur benefitsCompetitive salaryWe believe in recognizing the value of your skills and dedication, which is why we offer a salary that is aligned with industry standards. Your hard work will be fairly rewarded.Health packageYour well-being matters to us. Our robust health package includes a medical card, hospitalization coverage, and life insurance, providing you with peace of mind and support when you need it most.Device providedTo empower you in your role, we equip you with state-of-the-art tools. Enjoy the convenience of a company-provided MacBook Air or equivalent device.Transportation allowanceWe understand that commuting can be a challenge, so we offer a transportation allowance to make your daily journeys more convenient and affordable.Training sponsorshipWe believe in continuous learning and development. As part of our commitment to your professional growth, we provide sponsorship opportunities for industry-related training, helping you stay ahead of the curve and broaden your skill set.Exclusive merchandiseAs a valued member of our team, you'll have exclusive access to our sought-after CHIP merchandise. Show off your company pride with our unique collection of branded items.Job openingsSenior Developer (Golang)EngineeringTTDI, Kuala LumpurFull-timeApplyON HOLDCompliance OfficerOperationsTTDI, Kuala LumpurFull-timeApplyON HOLDProduct Manager (Fintech Solutions)EngineeringTTDI, Kuala LumpurFull-timeApplyON HOLDJunior Back End DeveloperEngineeringTTDI, Kuala LumpurFull-timeApplyON HOLDSenior Developer (Javascript)EngineeringTTDI, Kuala LumpurFull-timeApplyON HOLDMerchant Service Representative (Support)SalesTTDI, Kuala LumpurFull-timeApplyON HOLDMerchant Service Representative (Operations)SalesTTDI, Kuala LumpurFull-timeApplyON HOLDMerchant Acquiring RepresentativeSalesTTDI, Kuala LumpurFull-timeApplyON HOLDBusiness AnalystBusiness DevelopmentTTDI, Kuala LumpurFull-timeApplyCLOSEDOffice AdministratorPeopleTTDI, Kuala LumpurFull-timeApplyCLOSEDCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"30d1581bb93a26a84f37cd8ddad2a459-e0e3e7a2dda93e30-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=30d1581bb93a26a84f37cd8ddad2a459,sentry-sample_rate=1,sentry-transaction=GET%20%2Fcareers,sentry-sampled=true"}},"page":"/careers","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://portal.chip-in.asia/login</t>
   </si>
   <si>
@@ -94,6 +121,9 @@
     <t>CHIP Referral Program - Earn money with us</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact salesReferrer LoginJoin nowBecome our referral partnerLet's CHIP in our efforts to help merchants grow their businesses with us.Join nowContact salesAlready a referral partner? Login herePerks in becoming our partnerIn addition to the financial benefits, CHIP Referral Partners will also enjoy other exclusive benefits from us.Sales KitOngoing TrainingExclusive MerchandiseConferences and eventsHow to refer?Referring is easy! Simply share your referral link with your network OR introduce them to us. Start referring today and start earning!1. Register as a ReferrerSign up and become a referrer with us to start sharing your referral link and earning rewards. It’s free to join - no minimum refers.2. Share Referral linkShare your unique referral link with anyone looking for payment solution such as business owner who are looking for a Point-of-Sale machine.3. Start earningLogin to our Referral Portal (coming soon) to keep track of every successful referral and rewards earned. We offer flexible payment options.Referral commissionsEnjoy a standard commission rate below. Our settlements is on monthly basis.Let's discuss if you have a special project in mind.FPX Online BankingRM0.05* per paid transaction*Subject to final approvalB2C &amp; B2B1Credit and Debit Cards (Foreign &amp; Local)0.10%* per paid transaction*Subject to final approvalOn-Premise POS Terminal0.10%* per paid transaction*Subject to final approvalLocal &amp; Foreign Card/E-Wallets &amp; DuitNowComing soonBecome our Referral PartnerApply now or contact us at info@chip-in.asiaJoin nowContact salesAlready a referral partner? Login hereCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"b93e926ca18055c5c5702cbc0a457edd-63f752efecfb411a-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=b93e926ca18055c5c5702cbc0a457edd,sentry-sample_rate=1,sentry-transaction=GET%20%2Freferrer,sentry-sampled=true"}},"page":"/referrer","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://referrer.chip-in.asia/</t>
   </si>
   <si>
@@ -118,6 +148,9 @@
     <t>CHIP Brand Guidelines</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowBrand GuidelinesThis simple kit is for using the CHIP logo that follows our brand guidelines.Download kitZIP file contain PNG and SVG filesMain LogoThe CHIP logo consist of a "Symbol" and "Wordmark". The Symbol is inspired by the shape of chip on credit card.This is our primary logo. Note the "Symbol" and "Wordmark" are horizontally locked.When the primary logo doesn't fit in tight space, use the "Symbol" logo instead.ClearspaceOur logo should always have enough breathing space around it when placing beside another logo or text.We call the space around our logo the red zone. Do not put anything in it.ColourOn light background, use our full-colour primary logo. Purple hex code: #5147DDDark purple hex code: #140F37On darker background, use our full-colour primary logo with white (#FFFFFF) "CHIP" wordmark.Our CHIP purple is our identity, when working on dark background in tight space, use our purple coloured "Symbol".Printing only one colour? Use our black logo.On vibrant coloured background, use our white logo.On coloured background that clashed with our purple colour, use our white logo.Pay with CHIP badgesEnhance your customers' checkout experience with the "Pay with CHIP" badges. By displaying these badges, you show your commitment to providing a secure and trustworthy payment environment. Your customers can proceed to checkout with confidence, knowing that their preferred payment method meets our rigorous standards for safety and reliability.Payment via FPX (Online Banking).Payment via Foreign and Local Cards.Payment via DuitNow.Payment via E-Wallets.Generic "Pay with CHIP".Generic "Pay with CHIP" and "Powered by CHIP" can be used at your website footer.Payment via FPX(Online Banking) and all payment methods.Logo don'tsDo not stack the "Symbol" and "Wordmark".Do not change the CHIP purple colour.Do not change the shape of "Symbol"Do not swap position of the "Symbol" and "Wordmark".We know the "Symbol" looks like a chip, but do not replace it with an actual chip. 😬Kindly refrain from using grayscale version of the logo.We love gradients but do not use other than CHIP purple as the background of our logo.Do not use gradient on the "Wordmark".Do not add special effect such as drop shadow and outline on our logo.CHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"64735a39063dac57beef75b980112c71-314793bb49af3f18-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=64735a39063dac57beef75b980112c71,sentry-sample_rate=1,sentry-transaction=GET%20%2Fbrand,sentry-sampled=true"}},"page":"/brand","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://drive.google.com/uc?export=download&amp;id=194p1SW5cuBj2mxLF_sCKMHX568Vy_OMU</t>
   </si>
   <si>
@@ -127,6 +160,9 @@
     <t>CHIP 4K Wallpapers</t>
   </si>
   <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart Now4K WallpapersElevate your home screen with CHIP wallpapers.Desktop 16:9DownloadDownloadDownloadPhone 19:9DownloadDownloadDownloadCHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"4b55b988b20016c7e89610238debb1ae-1595caf19ab73925-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=4b55b988b20016c7e89610238debb1ae,sentry-sample_rate=1,sentry-transaction=GET%20%2Fwallpaper,sentry-sampled=true"}},"page":"/wallpaper","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
+  </si>
+  <si>
     <t>https://www.chip-in.asia/images/wallpaper/CHIP-wallpaper-desktop-1.jpg</t>
   </si>
   <si>
@@ -166,6 +202,9 @@
     <t>Terms of Service | CHIP - The Ultimate Digital Finance Platform for Your Business</t>
   </si>
   <si>
+    <t xml:space="preserve">Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowIntroductionOur ServicesData PrivacyOnboarding, Account and SecurityMerchant ObligationsTransaction, Authorisation &amp; SettlementService fees, Disputed Transactions &amp; RefundsSite and Community Platform RulesYour Content Contribution to the SiteDisclaimersExclusions and Limitations of LiabilityYour Representations and WarrantiesIndemnityRight of TerminationSuspensionSeverabilityGoverning LawGeneral ProvisionsDefinitions &amp; InterpretationsTerms of Service1. INTRODUCTION1.1.  Welcome to the Chip (accessible at https://www.chip-in.asia/) ("Site"). Please read the following Terms of Service carefully before using this Site or opening a Chip account ("Account") for the use of our Services (defined hereinafter) so that you are aware of your legal rights and obligations with respect to Chip In Sdn. Bhd. (Company No.: 202201010914 (1456611H))and its affiliates and subsidiaries (individually and collectively, "CHIP", "we", "us" or "our").1.2.  Before using our Services (defined hereinafter), you must read and accept all of the terms and conditions in, and linked to, our Terms of Service. In addition, you must consent to the processing of your personal data as described in the Privacy Policy linked hereto.1.3.  Chip reserves the right to change, modify, suspend or discontinue all or any part of our Site or Services at any time or upon notice as required by local laws. Chip may release certain services or their features in a beta version, which may not work correctly or in the same way the final version may work, and we shall not be held liable in such instances. Chip may also impose limits on certain features or restrict your access to parts of, or the entire, Site or Services in its sole discretion and without notice or liability.1.4.  Chip reserves the right to refuse to provide you access to our Site or Services or to allow you to open an Account with us for any reason.BY USING CHIP’S SERVICES OR OPENING AN ACCOUNT WITH CHIP, YOU GIVE YOUR IRREVOCABLE ACCEPTANCE OF AND CONSENT TO THE TERMS OF THIS AGREEMENT, INCLUDING THOSE ADDITIONAL TERMS AND CONDITIONS AND POLICIES REFERENCED HEREIN AND/OR LINKED HERETO. IF YOU DO NOT AGREE TO THESE TERMS, PLEASE DO NOT USE OUR SERVICES OR ACCESS THE SITE.2. OUR SERVICES2.1. The "Services" we provide or make available include:a. our Site;b. our System;c. our Community Platform;d. the payment gateway solutions to be integrated into your Website;e. the processing of Online Payment(s) made by your Customers for the purchase of your goods and/or services on your Website through our System for any Transactions;f. the processing of Offline Payment(s) made by your Customer for the purchase of your goods and/or services at your outlet through the use of Terminal for any Transactions;g. our expense and treasury management services;h. our data analytics services;i. services related to settlement to you with respect to such Transaction and the routing of Transactions by us for authorization, clearing and/or settlement purposes directly with the relevant Payment Scheme or via the Third Party Payment Partner; andj. all other services, software, and mobile application that we may offer from time to time.2.2. This Terms of Service shall govern your use of our Services.2.3.  Any new features added to or augmenting the Services and any software provided by us to you as part of the Services is subject to the Terms of Service. We reserve all rights to the software not expressly granted by us hereunder.2.4.  For the avoidance of doubt, any third-party scripts or code, linked to or referenced from the Services, are licensed to you by the third parties that own such scripts or code, not by us.2.5. For clarification purposes, when providing our Services, we are not to be construed as owing any fiduciary duty to you in respect of the payments made by your Customers through our System.3. DATA PRIVACY3.1.  Your privacy is very important to us at Chip. To better protect your rights, we have provided our Privacy Policy to explain our privacy practices in detail. Please review the Privacy Policy to understand how Chip collects and uses the information associated with your Account and/or your use of our Services. By using the Services or providing information to us, you consent to Chip’s collection, use, disclosure and/or processing of your personal data and User Information as described in the Privacy Policy. Please read the Privacy Policy carefully to better understand your legal rights and obligations in respect of data privacy.3.2.  When we process your Personal Data, we will do so in accordance with the Personal Data Protection Act 2010 (“PDPA”). Personal Data shall have the meaning as set out under the PDPA. We will only process Personal Data received from you for the purpose of and in connection with this Terms of Service and shall not further process the Personal Data in any manner incompatible with that purpose.4. ONBOARDING, ACCOUNT AND SECURITY4.1.  You will be able to access our Services through our Site by registering as an organisation representative (acknowledgement from your organisation is required to confirm your authority to act for your organisation). You will then be required to register for an Account by selecting a unique user identification ("User ID") and password, and by providing certain personal information.4.2.  In addition, you will be (and continue to be) subjected to our customer due diligence and know your customer (“KYC”) procedure before we may onboard you or continue to provide our Services to you. In connection with this, you hereby authorize us to conduct background checks on you through any credit reporting agency registered under the Credit Reporting Agencies Act 2010 as part of our KYC procedure and in compliance with the Anti-Money Laundering, Anti-Terrorism Financing and Proceeds of Unlawful Activities Act 2001 (“AMLA”). The background checks will include but are not limited to, credit checks, politically exposed persons (“PEP”), sanctions checks, adverse media checks, identity of your parent company , subsidiaries, directors, shareholders and ultimate beneficial owner. You are required, upon our request and from time to time, to provide us with information and/or copies of documents relating to, amongst others, your corporate structure, incorporation and statutory documents, and nature of business as part of our KYC procedure.4.3.  You may be able to use your Account to gain access to other products, websites or services to which we have enabled access or with which we have tied up or collaborated. Chip has not reviewed, and assumes no responsibility for any third-party content, functionality, security, services, privacy policies, or other practices of those products, websites or services. If you do so, the terms of service for those products, websites or services, including their respective privacy policies, if different from our Terms of Service and/or Privacy Policy, may also apply to your use of those products, websites or services.4.4.  You agree to (a) keep your password confidential and use only your User ID and password when logging in, (b) ensure that you log out from your account at the end of each session on the Site, (c) immediately notify Chip of any unauthorised use of your Account, User ID and/or password, and (d) ensure that your Account information is accurate and up-to-date. You are fully responsible for all activities that occur under your User ID and Account even if such activities or uses were not committed by you. Chip will not be liable for any loss or damage arising from the unauthorised use of your password or your failure to comply with this section.4.5. You agree that Chip may for any reason, in its sole discretion and with or without notice or liability to you or any third party, immediately suspend, freeze or terminate your Account and your User ID, remove or discard from the Site any Content associated with your Account and User ID, withdraw any subsidies offered to you, cancel any Transactions associated with your Account, temporarily or in more serious cases permanently withhold any Transactions, and/or take any other actions that Chip deems necessary. Grounds for such actions may include, but are not limited to, actual or suspected (a) extended periods of inactivity, (b) violation of the letter or spirit of these Terms of Service, (c) illegal, fraudulent or abusive behaviour, (d) abnormal transaction or activity, (e) violation of the terms and conditions of the TPPP and/or Payment Scheme, or (h) behaviour that is harmful to the business interests of Chip. In addition, the use of an Account for illegal, fraudulent or abusive purposes may be referred to law enforcement authorities without notice to you. If a legal dispute arises or law enforcement action is commenced relating to your Account or your use of the Services for any reason, Chip may terminate your Account immediately with or without notice.5. MERCHANT OBLIGATIONS5.1. You hereby undertake that you shall not perform any act in violation of the laws of Malaysia as well as the laws of any jurisdiction where you conduct business.5.2. You hereby agree that any successful Transactions conducted by any third party via fraudulent and illegal means are beyond our control and you agree to indemnify us in the event of any loss suffered by us in accordance with Clause 13 - Indemnity.5.3.  You hereby agree that we may from time to time require you and you shall perform payment verification with your Customer and/or the relevant Payment Channel operator in the event we suspect that the genuineness of the Transaction performed on your website and/or whenever such relevant Payment Channel operator so requires.5.4.  You hereby warrant that all information provided to us in connection with your application for the use of Services is correct and that no information has been withheld which, if provided, could have materially affected our decision to enter into this Terms of Service with you. For the avoidance of doubt, you shall immediately notify us if there are any changes to the above-required information.5.5.  You shall describe accurately on your Website, including a full description of your trading name, address, telephone number and URL, what goods and services are being offered for sale, the price, the action which must be taken to make a purchase, the point at which a sale is completed, and details of delivery, shipping, returns and refund policies.5.6.  You acknowledge and understand that Chip only grants you a limited and revocable license to access and use its Services subject to the terms and conditions herein. All proprietary Content, trademarks, service marks, brand names, logos and other intellectual property (“Intellectual Property”) displayed on the Site are the property of Chip and where applicable, third-party proprietors identified in the Site. No right or licence is granted directly or indirectly to any party accessing the Site to use or reproduce any Intellectual Property, and no party accessing the Site shall claim any right, title or interest therein.5.7.  By using or accessing the Services, you hereby agree to comply with the copyright, trademark, service mark, and all other applicable laws that protect the Services, the Site and its Content. You agree not to copy, distribute, republish, transmit, publicly display, publicly perform, modify, adapt, rent, sell, or create derivative works of any portion of the Services, the Site or its Content. You also may not, without our prior written consent, mirror or frame any part or whole of the Site on any other server or as part of any other website. You agree that you will not use any robot, spider or any other automatic device or manual process to monitor or copy the Site, its Content or its activities, without our prior written consent.5.8.  By using the Services and unless you expressly indicate otherwise, you hereby agree and authorise Chip to display your name, logo and/or trademark on its Site and marketing materials. For the avoidance of doubt, such use of name, logo and/or trademark will be limited to indicate that you are a client of Chip only.5.9.  You shall retain copies of all Transaction receipts, with respect to Transactions, for a period of seven (7) years and provide such copies of the Transaction receipts to us within five (5) Business Days upon receipt of such request to do so from us and hereby authorize us to transfer such information to the relevant Payment Channel operator required for the purposes of providing the Services to you.5.10.  In addition, you shall advise us as soon as you become aware of major or multiple product defects or logistics problems which could give rise to Charge Back or Refunds or any failure in delivering your goods and services to your Customer upon completing the Transaction.5.11. You shall be solely responsible for resolving directly with your Customer, any claims or complaints made by your Customer in respect of any purchase of goods, products or services made through our System and we shall not in any way be involved and responsible in the event your Customer disputes the underlying contract of sale for such Transaction for reasons including but not limited to the quality, overcharging or late delivery, of that good, product or service.5.12.  You undertake not to use our System to perform any transaction involving prohibited or restricted items under applicable laws, including but not limited to those listed as Banned Items.5.13. You acknowledge that to the extent that is applicable, Chip may be required to adhere to the additional terms and conditions implemented by the applicable laws, TPPP, Payment Scheme and/or Payment Channel, as and when it is informed to Chip. Where applicable, you agree to be bound by the additional terms and conditions of the TPPP, Payment Scheme and/or Payment Channel. Your continuing use of such Payment Channel constitutes your consent and agreement to such additions, removals and amendments to the additional terms and conditions of the TPPP, Payment Scheme and/or Payment Channel. For the avoidance of doubt, if there are any inconsistencies between the terms and conditions of the TPPP, Payment Scheme and/or Payment Channel and this Terms of Service, the specific terms and/or definitions in the TPPP, Payment Scheme and/or Payment Channel shall prevail with respect to the Payment Channel used by you.5.14. You shall establish and maintain adequate internal procedures and protocols to comply with the relevant Payment Channel standards as may be prescribed by the relevant TPPP, Payment Scheme and/or Payment Channel from time to time to mitigate the risk of Transaction fraud. For the purpose of this clause, “standards” means any laws, bylaws, rules, policies and operating regulations and procedures of the relevant TPPP, Payment Scheme and/or Payment Channel, including but not limited to any manuals, guides or bulletins, as may be amended from time to time.6. TRANSACTION, AUTHORISATION &amp; SETTLEMENT6.1.  The acceptance and processing of Transaction(s) shall not in any way be binding on us and we shall not honour any Transaction(s) which in our opinion is not genuine.6.2.  Authorization of a transaction does not guarantee payment to you nor is it a guarantee that it will not be subject to a Charge Back or other rights of reduction or set-off under this Terms of Service in relation to such Transaction.6.3.  For the purpose of authorization of Transactions, Chip may at its sole discretion route the Transactions directly to its designated Payment Scheme or Third Party Payment Partner.6.4.  Subject to Clause 6.5 and Clause 7, we will remit the payment of the Settlement Funds to your designated bank account in respect of each completed Transaction.6.5.  Notwithstanding anything contained herein, the amount of Settlement Funds due in respect of Transactions shall be deducted for the followings:6.5.1.  The Service Charges due as described in Clause 7;6.5.2.  Refunds in accordance with Clause 7;6.5.3.  Charge Back, fines and penalties passed on to us by the TPPP and/or Payment Scheme in respect of your Transactions;6.5.4.  Disputed Transactions and any amounts required to cover potential or expected Refunds, Charge Back or Disputed Transactions;6.5.5.  Any applicable taxes (including Sales and Service Tax at 6%), assessments or duties that may be introduced by the relevant authorities, which may vary from time to time;6.5.6.  Withholding tax (both domestic and international Payment Channels);6.5.7.  Foreign telegraphic transfer fee for overseas bank account settlement and foreign Payment Channels; and/or6.5.8.  Foreign exchange rate fluctuation (forex conversion for international Payment Channels).6.6.  If the settlement is below the minimum settlement amount, such settlement shall be carried forward to the next settlement date. In the event that the value of all items listed in Clause 6.5.1 to 6.5.8 exceeds the value of all Transactions falling due for settlement on the day due for settlement, the resulting shortfall may be held over by us for deduction against the following settlement when it shall be deducted from that settlement together with any interest due. Notwithstanding anything contained herein, we reserve the right at any time to require payment (including by directly debiting the charges to your account balances) of all or part of such shortfall in such currency as we may determine.6.7.  Settlement payment by us to you shall be in the settlement currency of Ringgit Malaysia and all foreign currencies will be converted to the currency of Ringgit Malaysia. We shall use the respective local bank’s prevailing bank exchange rates as the conversion rates.6.8.  We may hold back from the settlement any amounts reasonably required to cover potential or expected Refunds, Charge Back, or Disputed Transactions.7. SERVICE FEES, DISPUTED TRANSACTIONS &amp; REFUNDS7.1. In consideration of us providing the Services to you, you agree to pay us the Service Fees consisting of the following (where applicable):7.1.1.  A non-recurring and non-refundable Signup Fee;7.1.2.  A recurring and non-refundable Maintenance Fee payable annually;7.1.3.  The Transaction Fee on each Transaction and deduct the same from the payment made by the Customer in respect of each Transaction for the respective Payment Channels provided;7.1.5.  Telegraphic transfer charges per transfer charged by the financial institution;7.1.6.  Refund Service Fee on each refund request for the respective Payment Channels provided; and7.1.7.  The fee on Charge Back for each Charge Back transaction for the respective Payment Channels.7.2.  The chargeable amount of Service Fees shall follow the price list set out in our pricing email to you during your onboarding process and/or your Account’s dashboard. In the event of inconsistency between the price list of the two, the price list listed in your Account’s dashboard shall always prevail and be deemed conclusive.7.3.  We reserve the right to recover Service Fees provided in Clause 7.1.1 to 7.1.7 hereof by debiting your account balances if there is an insufficient fund available from your next settlement. Without prejudice to our other rights, we may suspend or withdraw the Services if our Service Fees or any other sums payable to us are not paid when due. You shall also be responsible for our additional costs in respect of dealing with your Customer disputes, Refunds, Charge Back, Disputed Transactions or other causes.7.4.  We reserve the rights to suspend you and withhold settlement to you in the event that the Maintenance Fee, Charge Back, and other due charges are not settled by you after one (1) week from the date the amount is due. Your account shall be reactivated upon settlement of all dues within one (1) Business Day.7.5.  By using our Services, you agree to pay us a security deposit(s). We shall have the right, in our sole discretion, to adjust the amount(s) held as we deem necessary as security against future Charge Back and shall notify you prior to such adjustments. In the event of any potential future payment disputes, Refunds or Charge Back in respect of your charges, we may also hold an adequate part of or all of the settlement’s amount in reserve to offset such disputed, refunded or Charge Backs amount plus any costs associated with the collection thereof, including without limitation, legal fees and expenses. We reserve the right to claim the payment from you if the reserve amount is inadequate to offset such disputed, refunded or Charge Back amount.7.6.  The maximum amount of any one settlement permitted under your account is referred to as the Trading Limit. We may vary the Trading Limit at any time by giving notice to you. We reserve the right to complete or reject any attempted payment that exceeds the applicable limit at our complete discretion. In addition, we reserve the right to further limit the amount or the frequency of transactions from your account for security reasons, and we shall not be liable to you if such a limitation is put in place. We reserve the right to refuse to honour payment requests that we believe or suspects are fraudulent or erroneous. You accept that we shall exercise this right at our sole discretion.7.7.  Notwithstanding anything contained herein, you agree that you shall not in any case rely upon us to discover or prevent loss as a result of fraud or erroneous payment and we shall not be responsible nor liable to you in the event a Customer disputes any Transaction.7.8.  We shall provide assistance with information regarding any Disputed Transaction, but we shall not be under any obligation or responsibility to investigate such disputed Transaction. The investigation of the Disputed Transaction or Charge Back on Transaction shall be performed by the Royal Police Malaysia, Cyber Crime Unit.7.9.  In the event of any Charge Back on Transaction made through Card, the Card Issuer’s decision shall be conclusive as to the determination of any Charge Back. Wherever possible (for example, if the TPPP provide us with written advice or upon us receiving notification from the Payment Scheme), notice to you of a Charge Back will be accompanied by an explanation of the reason for the Charge Back. Upon prior notification from us, we may debit your account, or otherwise, to recover any other costs and expenses we may incur as a result of or in connection with a Charge Back.7.10.  Where we are notified of any invalid or Disputed Transactions, we will notify you of the same by email and wherever possible (for example, if the TPPP provides us with written advise or upon us receiving notification from Payment Scheme) accompanied by an explanation of the reason for it. We will classify such Transaction as disputed and refer it back to you. You agree to investigate Disputed Transaction and take all reasonable steps to resolve disputes with the Customers within fourteen (14) days and follow the procedures for handling disputed Transactions and Charge Back which we shall advise from time to time. We shall have the right to suspend the processing of any Transaction or withhold settlement to you of the amount of that Disputed Transaction until the satisfactory completion of any investigation.7.11.  In the event that we consider in good faith there is a possibility of Charge Back, we shall have the discretion to retain the amount from any settlement (up to a maximum of 6 months) to cover the potential amount of such Charge Back and you shall on request provide such additional funds within one (1) week from the official request as we may specify in good faith to cover any Charge Back and potential Charge Back.7.12.  Where there is any Transaction to be refunded to a Customer, the amount shall be debited from your account, and thereafter you shall advise us via your Account or by hand or post on your letterhead with the authorized person’s signature affixed thereto, confirming such Refund to be made to the Customer.7.13.  Refunds shall only be made to the Card or Customer’s Bank where the original Transaction or Bank Account was debited, as applicable and not to any other method. A Refund Service Fee shall be chargeable to you where applicable.7.14.  The request for Refund will only be entertained and processed in accordance with the timeline provided by the Payment Scheme or TPPP.8. SITE AND COMMUNITY PLATFORM RULES8.1. You may access the Services through the Site and also participate in Chip’s discussion forum hosted through the Site (“Community Platform”). By using the Site and participating in the Community Platform, you agree not to:i. upload, post, transmit or otherwise make available any Content that is unlawful, harmful, threatening, abusive, harassing, alarming, distressing, tortuous, defamatory, vulgar, obscene, libelous, invasive of another's privacy, hateful, or racially, ethnically or otherwise objectionableii. violate any laws, including without limitation any laws and regulation in relation to export and import restrictions, third party rights or ourprohibited and restricted items list (amended and updated from time to time);iii. use the Services or upload Content to impersonate any person or entity, or otherwise misrepresent your affiliation with a person or entity;iv. remove any proprietary notices from the Site;v. use the Services or upload Content in a manner that is fraudulent, unconscionable, false, misleading or deceptive;vi. take any action that may undermine the Site or the Community Platform;vii. attempt to decompile, reverse engineer, disassemble or hack the Services (or any portion thereof), or to defeat or overcome any encryption technology or security measures implemented by Chip with respect to the Services and/or data transmitted, processed or stored by Chip;viii. harvest or collect any information about or regarding other Account holders, including, without limitation, any personal data or information;ix. upload, email, post, transmit or otherwise make available any Content that you do not have a right to make available under any law or under contractual or fiduciary relationships (such as inside information, proprietary and confidential information learned or disclosed as part of employment relationships or under nondisclosure agreements);x. upload, email, post, transmit or otherwise make available any Content that infringes any patent, trademark, trade secret, copyright or other proprietary rights of any party;xi. upload, email, post, transmit or otherwise make available any unsolicited or unauthorised advertising, promotional materials, "junk mail", "spam", "chain letters", "pyramid schemes", or any other unauthorised form of solicitation;xii. upload, email, post, transmit or otherwise make available any material that contains software viruses, worms, Trojan-horses or any other computer code, routines, files or programs designed to directly or indirectly interfere with, manipulate, interrupt, destroy or limit the functionality or integrity of any computer software or hardware or data or telecommunications equipment;xiii. take any action or engage in any conduct that could directly or indirectly damage, disable, overburden, or impair the Services or the servers or networks connected to the Services;xiv. use the Services to intentionally or unintentionally violate any applicable local, state, national or international law, rule, code, directive, guideline, policy or regulation including, without limitation, laws and requirements (whether or not having the force of law) relating to anti-money laundering or counter-terrorism; xv. use the Services to violate the privacy of others or to "stalk" or otherwise harass another;xvi. infringe the rights of Chip, including any intellectual property rights and any passing off of the same thereof; andxvii. use the Services to collect or store personal data about other Site’s users in connection with the prohibited conduct and activities set forth above.8.2.  You understand that all Content, whether publicly posted or privately transmitted, is the sole responsibility of the person from whom such Content originated. This means that you, and not Chip, are entirely responsible for all Content that you upload, post, email, transmit or otherwise make available through the Site. You understand that by using the Site, you may be exposed to Content that you may consider being offensive, indecent or objectionable. To the maximum extent permitted by applicable law, under no circumstances will Chip be liable in any way for any Content, including, but not limited to, any errors or omissions in any Content, or any loss or damage of any kind incurred as a result of the use of, or reliance on, any Content posted, emailed, transmitted or otherwise made available on the Site.8.3.  You acknowledge that Chip shall have the right (but not the obligation) in their sole discretion to pre-screen, refuse, delete, stop, suspend, remove or move any Content, including without limitation any Content or information posted by you, that is available on the Site without any liability to you. Without limiting the foregoing, Chip shall have the right to remove any Content (i) that violates the Terms of Service; (ii) if we receive a complaint from another user; (iii) if we receive a notice or allegation of intellectual property infringement or other legal instruction or request for removal; or (iv) if such Content is otherwise objectionable. We may also block delivery of a communication (including, without limitation, status updates, postings, messages and/or chats) to or from the Services as part of our effort to protect the Services, Site or our users, or otherwise enforce the provisions of the Terms of Service. You agree that you must evaluate, and bear all risks associated with, the use of any Content, including, without limitation, any reliance on the accuracy, completeness, or usefulness of such Content. In this regard, you acknowledge that you have not and, to the maximum extent permitted by applicable law, may not rely on any Content created by Chip or submitted to Chip.8.4.  You acknowledge, consent to and agree that Chip may access, preserve and disclose your Account information and Content to any legal, regulatory, or governmental authority, the relevant rights owner, or other third parties if required to do so by law pursuant to an order of a court or lawful request by any governmental or regulatory authority having jurisdiction over Chip or in a good faith belief that such access preservation or disclosure is reasonably necessary to: (a) comply with legal process; (b) enforce the Terms of Service; (c) respond to claims that any Content violates the rights of third parties, including intellectual property rights; (d) respond to your requests for customer service; or (e) protect the rights, property or personal safety of Chip, its Site’s users and/or the public.9. YOUR CONTENT CONTRIBUTION TO THE SITE9.1. By submitting Content to the Site, you represent and warrant that you have all necessary rights and/or permissions to grant the relevant licenses to Chip. Y ou further acknowledge and agree that you are solely responsible for anything you post or otherwise make available on or through the Services, including, without limitation, the accuracy, reliability, nature, rights clearance, compliance with the law and legal restrictions associated with any Content contribution. You hereby grant Chip and its successors a perpetual, irrevocable, worldwide, non-exclusive, royalty-free, sub- licensable and transferable license to use, copy, distribute, republish, transmit, modify, adapt, create derivative works of, publicly display, and publicly perform such Content contribution on, through or in connection with the Services in any media formats and through any media channels, including, without limitation, for promoting and redistributing part of the Services (and its derivative works) without the need of attribution and you agree to waive any moral rights (and any similar rights in any part of the world) in that respect. You understand that your contribution may be transmitted over various networks and changed to conform and adapt to technical requirements.9.2. Any Content, material, information or idea you post on the Site or through the Services or otherwise transmit to Chip by any means (each, a "Submission"), is not considered confidential by Chip and may be disseminated or used by Chip without </t>
+  </si>
+  <si>
     <t>mailto:info@chip-in.asia</t>
   </si>
   <si>
@@ -173,6 +212,9 @@
   </si>
   <si>
     <t>Privacy Policy | CHIP - The Ultimate Digital Finance Platform for Your Business</t>
+  </si>
+  <si>
+    <t>Our ProductsCOLLECTPayment ServicesCONTROLExpense ManagementSendPayouts in real-timeExpenseTeam's Expenses ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementBlogAPICareersContact usContact usLog inStart NowScope of this privacy policyChanges to this privacy policyThe information we collect and how we collect itHow we use your personal dataSecurity practicesAdvertisingSharing of your personal dataCommunications from usThird party services on our servicesRetention of your personal dataTransfer your data overseasYour rightsContactPrivacy policyWelcome to CHIP! In this Privacy Policy, “CHIP”, “CHIP IN” “we”, “our” or “us” refers to CHIP IN SDN. BHD.  (Company No.: 202201010914 (1456611-H)), a private company limited by shares incorporated under the laws of Malaysia and having its registered address at 7-2,  Plaza Danau 2 Jalan 2/109F, Taman Danau Desa, 58100 Kuala Lumpur, W.P. Kuala Lumpur Malaysia. We value your privacy and this Privacy Policy informs you of your choices and our practices regarding any Personal Data you provide to us or that you generate through your use of our services (“our services”), including our website at chip-in.asia or https://www.chip-in.asia/ (“Website” or “our Website”).1. SCOPE OF THIS PRIVACY POLICYThis Privacy Policy applies to our services and is incorporated into and forms part of the Term of Service (“Terms”) that you have agreed to in order to use our services. Any terms used in this Privacy Policy will have the same meaning as the equivalent defined terms in the Terms, unless otherwise defined in this Privacy Policy or the context requires otherwise. Please note that:this Privacy Policy does not apply to Personal Data collected through third party services (including any third-party websites or mobile apps) that you may access through our services;in providing our services, we may collect, use, disclose and retain your Personal Data;we share your Personal Data with our affiliates, business partners and service providers in order to provide our services to you, to carry out our obligations and enforce our rights, and to carry out our business (as set out in the “Sharing of Your Personal Information” section below).you have rights that you may exercise in relation to your Personal Data and you may exercise these rights by contacting us through the methods set out in the “Your Rights” section below.Kindly read this Privacy Policy carefully as it is important for you to understand how we collect and use your Personal Data and how you may control it. By using our services, you agree that we may collect, use and process your Personal Data in accordance with this Privacy Policy, as revised from time to time. If you do not agree with this Privacy Policy, you must not use our services.2. CHANGES TO THIS PRIVACY POLICYWe may from time to time, at our sole and absolute discretion, revise or add specific instructions, policies and terms to this Privacy Policy where such revisions, instructions, policies and terms shall form part of this Privacy Policy.  Where there are any changes to this Privacy Policy, we will notify you (via our website, direct communication to you, or any other means which we deem appropriate). You agree that by continuing to use our services after any changes to this Privacy Policy, you are agreeing to the revised Privacy Policy.3. THE INFORMATION WE COLLECT AND HOW WE COLLECT IT In providing our services, we collect and process the following Information relating to you:“Personal Data”, such as any data or information, whether true or not, which is (a) about an individual who can be identified (i) from that data; or (ii) from that data and other information to which we have or are likely to have access and would include data in our records as may be updated from time to time, or (b) defined as “personal data” or “personal information” under Malaysia’s Personal Data Protection Act 2010 (“PDPA”) and its subsidiary legislations and regulations as may be amended from time to time. Personal Data we collect and process include Identity Data, Contact Data, Biometric Data, Location Data, Log Data Payment Data and Marketing and Communications Data;“Identity Data”, such as your name, gender, date of birth, identification/passport number, nationality and photocopy of identity document or passport that you upload when using our services;“Contact Data”, such as residential address, mailing address, email address and phone numbers;“Biometric Data”, such as facial images when you upload image or video of yourself when using our services;“Location Data”, such as information regarding your location (when you use a location-enabled services), including the location of your device when you use our services, such as from the GPS, WiFi, compass, accelerometer or other sensors in your device;"Log Data", such as technical information that is automatically collected when you use our services, including (a) technical information such as your mobile carrier, configuration information made available by your device, web browser or other programs you use to access our services, your IP address, mac address and your device’s type, model, version and identification number; and (b) information about your use of our services;“Marketing and Communications Data”, such as your preferences in receiving marketing information from us, our affiliates, business partners and service providers, and your communication preferences; and“Payment Data”, such as your bank account, payment information and your transactional data.You must only submit Personal Data which is accurate and not misleading and you must keep it up to date and inform us of any changes to the Personal Data you have provided to us. We shall have the right to request for documentation to verify the Personal Data provided by you as part of our customer due diligence processes. We disclaim any liability for failure to provide services to you if you fail to ensure that your Personal Data submitted to us is complete and accurate. You may access and update your Personal Data submitted to us at any time by contacting us using the details set out in the “Contact” section below.‍4. HOW WE USE YOUR PERSONAL DATAWe may use your Personal Data for any of the following purposes:to provide our services to you;to consider and process your transaction or communications with third parties via our services;for identification, verification, due diligence, or know your customer purposes;to respond to, process, deal with or complete a transaction and/or to fulfil your requests for certain products and services and notify you of service issues and unusual account actions;to enforce our Terms or any applicable end user agreements, merchant agreements and/or license agreements;for customer service, security, fraud-detection, archival and backup purposes in connection with the provision of our services;to better understand how you access and use our services, for the purposes of trying to improve our services and to respond to customer desires and preferences, including language and location customisation, personalised help and instructions, or other responses to your and other clients’ usage of our services;to carry out due diligence or other screening activities (including, without limitation, background checks) in accordance with legal or regulatory obligations or our risk management procedures that may be required by law or that may have been put in place by us;to audit our services and business;to prevent or investigate any actual or suspected violations of our Terms, fraud, unlawful activity, omission or misconduct, whether relating to your use of our Services or any other matter arising from your relationship with us;to respond to any threatened or actual claims asserted against us;to store, host, back up (whether for disaster recovery or otherwise) of your personal data, whether within or outside of your jurisdiction;to help us develop our new services and/or improve our existing services;software verification or administering software upgrades;our business and commercial transactions; and/orany other purposes which we notify you of at the time of obtaining your consent.Please note that as the purposes for which we will/may collect, use, disclose or process your Personal Data depend on the circumstances at hand, such purpose may not appear above. However, we will notify you of such other purpose at the time of obtaining your consent, unless processing of the applicable data without your consent is permitted by the applicable laws or regulations.If we rely on your consent for us to use your Personal Data in a particular way, but you change your mind, you may withdraw your consent by contacting us using the details set out in the “Contact” section below. Upon the receipt of such withdrawal notice from you, we will stop such use of your Personal Data. However, if you withdraw your consent, this may impact our ability to provide you with our services.5. SECURITY PRACTICESWe use a variety of security technologies and procedures for the purpose of preventing loss, misuse, unauthorised access or disclosure of your Personal Data. We use Secure Socket Layer (SSL) technology to store your Personal Data.6. ADVERTISINGIn the event that we use your Personal Data for advertising purposes, we will do so in accordance with this section. We may use your Personal Data to try to offer advertising that is more relevant to you. We may also use your Personal Data for the purpose of sending you direct marketing information or materials (whether by messaging within our services or by other means) that offer or advertise our products and/or services and/or the products and/or services of selected third parties including our affiliates, business partners and service providers.We will honour your request for us to not use your Personal Data for the marketing purposes as described above. If you wish to make such a request, please: (a) contact us by using the details set out in the “Contact” section below; (b) follow the relevant instructions on our marketing communications; or (c) follow the instructions as set out in certain service-specific guidance (in relation to the relevant service).Please note that we do not share your Personal Data with advertisers. We may, however, share Personal Data that cannot be used to identify you in aggregated, anonymised or pseudonymised form with advertisers for the purposes of trying to offer you advertising that is more relevant to you.7. SHARING OF YOUR PERSONAL DATAUnless permitted under this Privacy Policy or otherwise consented by you, we will not transfer your Personal Data to any third parties except our affiliates, business partners and service providers where such affiliates, business partners and service providers may collect your Personal Data across our services.Any collection and/or sharing of your Personal Data as permitted under the provision above or any other provisions of this Privacy Policy will only be used for the purposes of:providing our services to you;assisting us in carrying out the purposes set out under the “How We Use Your Personal Data” section above;carrying out our obligations and enforcing our rights under the Terms or this Privacy Policy; and/orour businesses, including helping us to understand our client/user better and/or to improve our services.Where we permit any third parties to collect and use your Personal Data in accordance with the provisions above, we will use reasonable efforts to ensure that such third parties only use your Personal Data: (i) in compliance with this Privacy Policy; and (ii) subject to any other instructions we give them, including any appropriate confidentiality and security measures that we implement. You hereby consent to the third-party use and sharing of your Personal Data as described in this "Sharing of your Personal Data" section.Under specific circumstances, you agree that we may be required to retain, preserve or disclose your Personal Data to comply with any legal requirements, including:in order to comply with applicable laws or regulations or where we believe it is reasonably necessary to comply with the applicable laws or regulations;in order to comply with a court order or other legal process; and/orin response to a request by a government authority, law enforcement agency or similar body (whether situated in your jurisdiction or elsewhere).8. COMMUNICATIONS FROM USWhen you use our services, we may send you notifications through our website and our mobile app installed on your device (if applicable). If you no longer wish to receive these communications, you can do so by opting out of notifications at the website user account level or device level. We may from time to time send you service-related announcements when we consider it necessary to do so (such as when we temporarily suspend one of our services for maintenance). You may not opt-out of these service-related announcements, which are not promotional in nature.9. THIRD PARTY SERVICES ON OUR SERVICESOur services may include, or they may link you to, social media or other services (including websites) provided by third parties. For example, we may (whether in advertisements or otherwise within our services) provide you with links that allow you to access third party services or websites. Your use of any such third-party services, including any Personal Data you provide to such third parties, are subject to the relevant third party’s own terms of services and privacy policies and not our Terms or this Privacy Policy, so please review their terms carefully. This Privacy Policy only applies to any Personal Data collected by us, does not apply to any Personal Data collected by such third parties or services offered by such third parties, and we bear no liability for any third-party use of any Personal Data provided by you to them.10. RETENTION OF YOUR PERSONAL DATAWe retain your Personal Data only if we need it to support justifiable business requirements or if required by the applicable laws. For example, we will only retain your Personal Data for as long as we have a business relationship with you and for a period of time afterwards where we have an ongoing business need to retain it, or where we are required by law to retain it. Upon the expiry of time relating to any business needs or legal requirements to retain your Personal Data, we will take reasonable step to ensure that your Personal Data is deleted or anonymised.11. TRANSFER YOUR DATA OVERSEASYour Personal Data will be processed in Malaysia, where our servers are located.12. YOUR RIGHTSYou have the right to request access to Personal Data that we hold about you, subject to certain conditions and limited exceptions set out in the applicable laws. If you wish to do so, please email your request to us by using the details set out in the “Contact” section below.We will be as open as we can with you but sometimes we might not hold any Personal Data about you or may have to withhold Personal Data from you, but only to the extent we are allowed to do so under the applicable laws. For example, where the information is not Personal Data about you, is commercially sensitive, is legally privileged or relates to the Personal Data of another person, or disclosure of the information may have impact on the safety or security of our employees, clients or any person. In any of such circumstances, we may withhold the information requested by you and provide you with reason.You have the right to ask us not to use your Personal Data for marketing purposes or any other purpose. You can exercise the right at any time by contacting us using the details set out in the “Contact” section below.You may also have a right under the applicable laws to make other requests relating to your Personal Data. For example, you may have a right to:request that we update or correct the record of your Personal Data maintained by us if it is inaccurate or out of date;request that we erase that data or cease processing it, subject to certain exceptions;receive your Personal Data in a structured, commonly used and machine-readable format, and to transmit that data to another data controller; andlodge a complaint with the appropriate data protection authority if you have concerns about how we process your Personal Data.  Alternatively, you may seek a remedy through the courts if you believe your rights have been breached.If you wish to exercise any of the above rights, please make your request by using the details set out in the “Contact” section below.13. CONTACTIf you wish to contact us regarding this Privacy Policy or to exercise your rights under the PDPA, please contact our Privacy Officer via email at info@chip-in.asia.Last Updated: 22 June 2022CHIP IN SDN. BHD. (202201010914 (1456611-H))Lot 3A-01A, Level 3AGlo Damansara Shopping Mall,699, Jalan Damansara, Taman Tun Dr Ismail60000 Kuala Lumpur, MalaysiaOffice line: (+60)3 2935 9253CHIP ProductsCOLLECTPayment ServicesSENDPayouts in real-timeEXPENSETeam Expense ManagementADVANCEPay-As-You-Sell Advance™COMPLIANCERisk ManagementCOINTreasury ManagementPartnersBecome a referral partnerReferrer LoginResourcesBlogAPICHIP Services StatusFPX Bank StatusCompanyInvestor RelationsContact usCareersBrand assetsDownload wallpaperFollow usTerms of Service · Privacy Policy · © 2025 CHIPChat with us{"props":{"pageProps":{"_sentryTraceData":"23df4e0a996763ddd026c6d5a11459d0-72d33a07543707ff-1","_sentryBaggage":"sentry-environment=production,sentry-release=jDsTDFf4g7e7OYWfH40gQ,sentry-public_key=55f8e3ef4da14d0501741236e07d0229,sentry-trace_id=23df4e0a996763ddd026c6d5a11459d0,sentry-sample_rate=1,sentry-transaction=GET%20%2Fprivacy-policy,sentry-sampled=true"}},"page":"/privacy-policy","query":{},"buildId":"jDsTDFf4g7e7OYWfH40gQ","isFallback":false,"isExperimentalCompile":false,"appGip":true,"scriptLoader":[]}</t>
   </si>
   <si>
     <t>https://api.whatsapp.com/send?phone=60149362105&amp;text=Hi%20CHIP.</t>
@@ -611,7 +653,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="2" min="1" width="100"/>
+    <col customWidth="true" max="3" min="1" width="80"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -621,645 +663,888 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C60" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C61" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C68" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C69" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C72" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C73" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B75" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C78" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C79" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C80" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C81" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>